<commit_message>
added packages NOTE: Delete dumy Classes
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_grp_blue.xlsx
+++ b/doc/task10/scrum_grp_blue.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -244,15 +244,6 @@
   </si>
   <si>
     <t>Controller</t>
-  </si>
-  <si>
-    <t>Testing the first Sprint</t>
-  </si>
-  <si>
-    <t>Testing the Object of the first Sprint</t>
-  </si>
-  <si>
-    <t>Tests</t>
   </si>
   <si>
     <t>open</t>
@@ -791,7 +782,7 @@
       </c>
       <c r="E3">
         <f>SUM('Sprint Backlog'!I9:I13)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -855,7 +846,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -955,7 +946,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -978,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1001,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="58" x14ac:dyDescent="0.35">
@@ -1033,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1065,7 +1056,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -1097,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O8" s="2"/>
     </row>
@@ -1130,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -1162,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1194,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1226,40 +1217,11 @@
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>2.7</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="L13" t="s">
-        <v>77</v>
-      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated srum board (sprint log)
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_grp_blue.xlsx
+++ b/doc/task10/scrum_grp_blue.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>open</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -846,7 +852,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1024,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1056,7 +1062,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -1087,8 +1093,11 @@
       <c r="I8">
         <v>2</v>
       </c>
+      <c r="K8">
+        <v>0.33</v>
+      </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O8" s="2"/>
     </row>
@@ -1120,8 +1129,11 @@
       <c r="I9">
         <v>6</v>
       </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
@@ -1152,8 +1164,11 @@
       <c r="I10">
         <v>2</v>
       </c>
+      <c r="K10">
+        <v>0.33</v>
+      </c>
       <c r="L10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1184,8 +1199,11 @@
       <c r="I11">
         <v>2</v>
       </c>
+      <c r="K11">
+        <v>0.33</v>
+      </c>
       <c r="L11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -1217,7 +1235,7 @@
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
better descriptions for si taskas
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_grp_blue.xlsx
+++ b/doc/task10/scrum_grp_blue.xlsx
@@ -17,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +310,36 @@
   </si>
   <si>
     <t>Implement new Appointment Pop-Up UIController</t>
+  </si>
+  <si>
+    <t>Implementing the Pop-Up View for the new Appointment with the nessecairy fields</t>
+  </si>
+  <si>
+    <t>Implementing the functionality for the new Appointment function</t>
+  </si>
+  <si>
+    <t>Implementing some dummy Patients for the Patient List view</t>
+  </si>
+  <si>
+    <t>Plan the state event pattern for the Patient State</t>
+  </si>
+  <si>
+    <t>Implement the Pattient List View after hugil1 has designed it and made a prototype</t>
+  </si>
+  <si>
+    <t>Implementing the retrieve Patients functioanality for the Patient List view</t>
+  </si>
+  <si>
+    <t>Implementing the functions (logic) for the new Patient functionsality</t>
+  </si>
+  <si>
+    <t>Creating and Planing the GUI for the Patient List View and make a little prototype</t>
+  </si>
+  <si>
+    <t>Creating and Planing the GUI for the new Patient View with a little Prototype. IMPORTANT: DO SHOW ALL NECESSAIRY FIELDS!!</t>
+  </si>
+  <si>
+    <t>Implementing the popup with the necessairy fields for new Patients functionality</t>
   </si>
 </sst>
 </file>
@@ -926,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1391,7 +1421,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.1</v>
       </c>
@@ -1399,7 +1429,9 @@
       <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="E15" t="s">
         <v>72</v>
       </c>
@@ -1419,7 +1451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.2</v>
       </c>
@@ -1427,6 +1459,9 @@
       <c r="C16" t="s">
         <v>95</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E16" t="s">
         <v>73</v>
       </c>
@@ -1446,7 +1481,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4.0999999999999996</v>
       </c>
@@ -1454,6 +1489,9 @@
       <c r="C17" t="s">
         <v>78</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="E17" t="s">
         <v>71</v>
       </c>
@@ -1473,7 +1511,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4.2</v>
       </c>
@@ -1481,6 +1519,9 @@
       <c r="C18" t="s">
         <v>89</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E18" t="s">
         <v>77</v>
       </c>
@@ -1500,7 +1541,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>4.3</v>
       </c>
@@ -1508,6 +1549,9 @@
       <c r="C19" t="s">
         <v>88</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E19" t="s">
         <v>72</v>
       </c>
@@ -1527,7 +1571,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>4.4000000000000004</v>
       </c>
@@ -1535,6 +1579,9 @@
       <c r="C20" t="s">
         <v>87</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E20" t="s">
         <v>73</v>
       </c>
@@ -1554,18 +1601,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4.5</v>
       </c>
       <c r="C21" t="s">
         <v>90</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E21" t="s">
         <v>72</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>25</v>
@@ -1580,18 +1630,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>4.5999999999999996</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E22" t="s">
         <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
         <v>17</v>
@@ -1606,13 +1659,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>4.7</v>
       </c>
       <c r="C23" t="s">
         <v>79</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="E23" t="s">
         <v>72</v>
       </c>
@@ -1632,12 +1688,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4.8</v>
       </c>
       <c r="C24" t="s">
         <v>80</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="E24" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
some minor changes and add new patient with state
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_grp_blue.xlsx
+++ b/doc/task10/scrum_grp_blue.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1418,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="58" x14ac:dyDescent="0.35">
@@ -1447,8 +1447,11 @@
       <c r="I15">
         <v>6</v>
       </c>
+      <c r="K15" s="12">
+        <v>6</v>
+      </c>
       <c r="L15" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="58" x14ac:dyDescent="0.35">
@@ -1477,8 +1480,11 @@
       <c r="I16">
         <v>6</v>
       </c>
+      <c r="K16" s="12">
+        <v>6</v>
+      </c>
       <c r="L16" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1507,8 +1513,11 @@
       <c r="I17">
         <v>6</v>
       </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
       <c r="L17" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -1537,8 +1546,11 @@
       <c r="I18">
         <v>4</v>
       </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
       <c r="L18" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
@@ -1567,8 +1579,11 @@
       <c r="I19">
         <v>6</v>
       </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
       <c r="L19" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1626,8 +1641,11 @@
       <c r="I21">
         <v>6</v>
       </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
       <c r="L21" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1684,6 +1702,9 @@
       <c r="I23">
         <v>4</v>
       </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
       <c r="L23" s="12" t="s">
         <v>75</v>
       </c>
@@ -1712,6 +1733,9 @@
       </c>
       <c r="I24">
         <v>4</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>75</v>

</xml_diff>